<commit_message>
week4 kaggle baseline beaten
</commit_message>
<xml_diff>
--- a/6_Final_projects/2_churn_prediction/results.xlsx
+++ b/6_Final_projects/2_churn_prediction/results.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A1AAC6-98EA-4A5A-97AE-6649F020C52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>roc auc</t>
   </si>
@@ -79,12 +80,39 @@
   </si>
   <si>
     <t>0.49919</t>
+  </si>
+  <si>
+    <t>0.67713</t>
+  </si>
+  <si>
+    <t>0.7127077471277219</t>
+  </si>
+  <si>
+    <t>0.7090677210791867</t>
+  </si>
+  <si>
+    <t>0.004871442393976412</t>
+  </si>
+  <si>
+    <t>0.47916666666666663</t>
+  </si>
+  <si>
+    <t>0.0024509803921568627</t>
+  </si>
+  <si>
+    <t>scaler</t>
+  </si>
+  <si>
+    <t>StandardScaler</t>
+  </si>
+  <si>
+    <t>GradientBoostingClassifier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,7 +146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -150,7 +178,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2" descr="http://EC89718711D1234F9D3A7B3407D1F512.dms.sberbank.ru/EC89718711D1234F9D3A7B3407D1F512-86AB11783FAC1265EF5A2B999A130797-3DD10827110F3CD97C28DDE8BB3389AB/1.png"/>
+        <xdr:cNvPr id="3" name="Рисунок 2" descr="http://EC89718711D1234F9D3A7B3407D1F512.dms.sberbank.ru/EC89718711D1234F9D3A7B3407D1F512-86AB11783FAC1265EF5A2B999A130797-3DD10827110F3CD97C28DDE8BB3389AB/1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
@@ -438,36 +472,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B5:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.86328125" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="H5" t="s">
         <v>6</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -493,10 +529,13 @@
         <v>8</v>
       </c>
       <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -521,8 +560,40 @@
       <c r="I7" t="s">
         <v>10</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>